<commit_message>
Read research paper : Biodegardation of lipid -rich waste water by combination of microwave Irradiation and Lipase Immobilized on Chitosan (2006)
</commit_message>
<xml_diff>
--- a/res/data/Summary of Research Papers on LCFA inhibition.xlsx
+++ b/res/data/Summary of Research Papers on LCFA inhibition.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Research paper</t>
   </si>
@@ -31,6 +31,24 @@
   </si>
   <si>
     <t xml:space="preserve">Enzymatic pre-hydrolysis applied to the anaerobic treatment of effluents from poultry slaughterhouses </t>
+  </si>
+  <si>
+    <t>solid-state fermentation of the fungus Penicillium restrictum</t>
+  </si>
+  <si>
+    <t>Measured Parameters</t>
+  </si>
+  <si>
+    <t>Anaerobic digestion of lipid-rich waste — Effects of lipid concentration</t>
+  </si>
+  <si>
+    <t>Lipase 80,000 from Rhizopus oryzae</t>
+  </si>
+  <si>
+    <t>Methane Production/GC-VFA/ VS/initial VSS</t>
+  </si>
+  <si>
+    <t>COD/Oil and Grease/Biogas/Methane Production/Free fatty acids (titrimetric)/ VS/ initial VSS</t>
   </si>
 </sst>
 </file>
@@ -385,19 +403,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.85546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,13 +428,36 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>2007</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2006</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read research paper : Effect of enzymatic pretreatment on the anaerobic digestion of milk fat for biogas production
</commit_message>
<xml_diff>
--- a/res/data/Summary of Research Papers on LCFA inhibition.xlsx
+++ b/res/data/Summary of Research Papers on LCFA inhibition.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Research paper</t>
   </si>
@@ -49,6 +49,24 @@
   </si>
   <si>
     <t>COD/Oil and Grease/Biogas/Methane Production/Free fatty acids (titrimetric)/ VS/ initial VSS</t>
+  </si>
+  <si>
+    <t>Commercial Candida Rugosa lipase</t>
+  </si>
+  <si>
+    <t>Biodegradation of Lipid-rich Waste Water by Combination of Microwave Irradiation and Lipase Immobilized on Chitosan</t>
+  </si>
+  <si>
+    <t>Free fatty acids (titrimetric)/Enzyme activity</t>
+  </si>
+  <si>
+    <t>Effect of enzymatic pretreatment on the anaerobic digestion of milk fat for biogas production</t>
+  </si>
+  <si>
+    <t>Sigma Ladrich Candida Rugosa lipase</t>
+  </si>
+  <si>
+    <t>Methane Production/COD/Free fatty acids</t>
   </si>
 </sst>
 </file>
@@ -403,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,6 +478,34 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2006</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Read research paper : Pretreatment of Coconut Mill Effluent Using Celite-Immobilized Hydrolytic Enzyme Preparation from Staphylococcus pasteuri and Its Impact on Anaerobic Digestion
</commit_message>
<xml_diff>
--- a/res/data/Summary of Research Papers on LCFA inhibition.xlsx
+++ b/res/data/Summary of Research Papers on LCFA inhibition.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Research paper</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Methane Production/COD/Free fatty acids</t>
+  </si>
+  <si>
+    <t>Glycerol/Free fatty acids/Lipids/Proteins/Reducing sugars/Biogas/O&amp;G/COD</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +435,7 @@
     <col min="1" max="1" width="42.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.28515625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -506,6 +509,11 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Life Cycle Analysis : Model, Research Papers, Writing Paper
</commit_message>
<xml_diff>
--- a/res/data/Summary of Research Papers on LCFA inhibition.xlsx
+++ b/res/data/Summary of Research Papers on LCFA inhibition.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Research paper</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Glycerol/Free fatty acids/Lipids/Proteins/Reducing sugars/Biogas/O&amp;G/COD</t>
+  </si>
+  <si>
+    <t>Pretreatment of Coconut Mill Effluent Using Celite-Immobilized Hydrolytic Enzyme Preparation from Staphylococcus pasteuri and Its Impact on Anaerobic Digestion</t>
+  </si>
+  <si>
+    <t>Lipase from Staphylococcus pasteuri</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -509,7 +515,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>